<commit_message>
goal verify layout, change some stuff to allow fraction stuff, plan out goal verify
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE57C7FC-30CD-4765-93E0-0B131CBE5784}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5621A1-9485-471E-9AF9-67BECC39C5F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1215" yWindow="3615" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>Kero Builder</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>goal_height_req</t>
+  </si>
+  <si>
+    <t>Height:</t>
   </si>
 </sst>
 </file>
@@ -379,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +447,30 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some more goal evaluation stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5621A1-9485-471E-9AF9-67BECC39C5F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68358A6C-C5D9-45E5-9F99-895AA0654A2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="3615" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1845" yWindow="2685" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Key</t>
   </si>
@@ -62,6 +62,42 @@
   </si>
   <si>
     <t>Height:</t>
+  </si>
+  <si>
+    <t>Not enough volume!</t>
+  </si>
+  <si>
+    <t>Each object's height must be {0} tall!</t>
+  </si>
+  <si>
+    <t>goal_volume_req</t>
+  </si>
+  <si>
+    <t>Volume:</t>
+  </si>
+  <si>
+    <t>goal_total_volume</t>
+  </si>
+  <si>
+    <t>Total Volume:</t>
+  </si>
+  <si>
+    <t>goal_efficiency</t>
+  </si>
+  <si>
+    <t>Efficiency:</t>
+  </si>
+  <si>
+    <t>goal_error_not_found</t>
+  </si>
+  <si>
+    <t>No matching objects found!</t>
+  </si>
+  <si>
+    <t>goal_error_height_not_met</t>
+  </si>
+  <si>
+    <t>goal_error_volume_not_enough</t>
   </si>
 </sst>
 </file>
@@ -397,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +507,54 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
placeholder cube types, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68358A6C-C5D9-45E5-9F99-895AA0654A2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DF8893-A292-4743-A857-0B735021FEB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="2685" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Key</t>
   </si>
@@ -98,6 +98,36 @@
   </si>
   <si>
     <t>goal_error_volume_not_enough</t>
+  </si>
+  <si>
+    <t>cube_field</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>cube_pond</t>
+  </si>
+  <si>
+    <t>Pond</t>
+  </si>
+  <si>
+    <t>cube_house_1</t>
+  </si>
+  <si>
+    <t>cube_house_2</t>
+  </si>
+  <si>
+    <t>cube_house_3</t>
+  </si>
+  <si>
+    <t>House 01</t>
+  </si>
+  <si>
+    <t>House 02</t>
+  </si>
+  <si>
+    <t>House 03</t>
   </si>
 </sst>
 </file>
@@ -433,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +585,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
more hud art stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DF8D00-ABA8-4C1E-8BF1-D0B68C247820}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0040FA-316F-4BD1-92ED-4627E3AADACF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Key</t>
   </si>
@@ -182,6 +182,24 @@
   </si>
   <si>
     <t>OBJECTIVES</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>BUILD</t>
   </si>
 </sst>
 </file>
@@ -517,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,129 +643,153 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some refactors, art adjustments
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0040FA-316F-4BD1-92ED-4627E3AADACF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB55D9D-914A-479E-8885-99F826D0B670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Key</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>BUILD</t>
+  </si>
+  <si>
+    <t>victory_title</t>
+  </si>
+  <si>
+    <t>MISSION COMPLETE</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Score:</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,41 +767,57 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
level 3-5 background, level 3 and 4, hide volume displays, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB55D9D-914A-479E-8885-99F826D0B670}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3801C18-0944-4CD9-B8BD-32BA15E1073A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Not enough volume!</t>
   </si>
   <si>
-    <t>Each object's height must be {0} tall!</t>
-  </si>
-  <si>
     <t>goal_volume_req</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Score:</t>
+  </si>
+  <si>
+    <t>One or more objects do not match the height!</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,82 +599,82 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -695,21 +695,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -717,108 +717,117 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
level 7 stuff, change house icons, added ranking
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3801C18-0944-4CD9-B8BD-32BA15E1073A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C5726-7823-418F-9F18-B6E613BC0C08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -100,15 +100,9 @@
     <t>cube_field</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
     <t>cube_pond</t>
   </si>
   <si>
-    <t>Pond</t>
-  </si>
-  <si>
     <t>cube_house_1</t>
   </si>
   <si>
@@ -118,15 +112,6 @@
     <t>cube_house_3</t>
   </si>
   <si>
-    <t>House 01</t>
-  </si>
-  <si>
-    <t>House 02</t>
-  </si>
-  <si>
-    <t>House 03</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -212,6 +197,33 @@
   </si>
   <si>
     <t>One or more objects do not match the height!</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>Bonus:</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Pennyroyal House</t>
+  </si>
+  <si>
+    <t>Marigold House</t>
+  </si>
+  <si>
+    <t>Pleasant Field</t>
+  </si>
+  <si>
+    <t>Serene Pond</t>
+  </si>
+  <si>
+    <t>Green House</t>
   </si>
 </sst>
 </file>
@@ -547,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,82 +611,82 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -695,18 +707,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +769,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -776,58 +788,74 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
art stuff for start scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C5726-7823-418F-9F18-B6E613BC0C08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A3F88-5C57-456F-925B-A503845855A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Key</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>Green House</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>CREDITS</t>
+  </si>
+  <si>
+    <t>credits_detail</t>
+  </si>
+  <si>
+    <t>Written By: David Dionisio\nMusic From: Kevin Macleod</t>
   </si>
 </sst>
 </file>
@@ -559,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,250 +629,274 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some of level 0 tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A3F88-5C57-456F-925B-A503845855A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F35DE7-7091-4290-94D9-D91373221D4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="2565" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Key</t>
   </si>
@@ -242,6 +242,57 @@
   </si>
   <si>
     <t>Written By: David Dionisio\nMusic From: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>intro_0</t>
+  </si>
+  <si>
+    <t>Welcome to Kero Builder!</t>
+  </si>
+  <si>
+    <t>intro_1</t>
+  </si>
+  <si>
+    <t>intro_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will be playing as a builder to help these spacefaring frogs settle into their new planet. </t>
+  </si>
+  <si>
+    <t>Let's do our best to build their homes!</t>
+  </si>
+  <si>
+    <t>level_0_intro_0_1</t>
+  </si>
+  <si>
+    <t>Before we begin, let's first look at the view controls.</t>
+  </si>
+  <si>
+    <t>level_0_intro_0_2</t>
+  </si>
+  <si>
+    <t>You can drag the view around to get a better look at the map.</t>
+  </si>
+  <si>
+    <t>level_0_intro_0_3</t>
+  </si>
+  <si>
+    <t>next_instruct</t>
+  </si>
+  <si>
+    <t>Press this button when you're ready to continue.</t>
+  </si>
+  <si>
+    <t>These buttons allow you to rotate or elevate the view.</t>
+  </si>
+  <si>
+    <t>level_0_intro_1_1</t>
+  </si>
+  <si>
+    <t>The information on the upper-left tells you the measurement of the unit cube.</t>
+  </si>
+  <si>
+    <t>level_0_intro_1_2</t>
   </si>
 </sst>
 </file>
@@ -577,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +919,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -876,7 +927,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -884,7 +935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -892,12 +943,90 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more level 0 instructions
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F35DE7-7091-4290-94D9-D91373221D4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C598F135-A39E-4EA6-8210-4C150E3B4F3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Key</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Score:</t>
   </si>
   <si>
-    <t>One or more objects do not match the height!</t>
-  </si>
-  <si>
     <t>bonus</t>
   </si>
   <si>
@@ -280,12 +277,6 @@
     <t>next_instruct</t>
   </si>
   <si>
-    <t>Press this button when you're ready to continue.</t>
-  </si>
-  <si>
-    <t>These buttons allow you to rotate or elevate the view.</t>
-  </si>
-  <si>
     <t>level_0_intro_1_1</t>
   </si>
   <si>
@@ -293,6 +284,126 @@
   </si>
   <si>
     <t>level_0_intro_1_2</t>
+  </si>
+  <si>
+    <t>One or more builds do exceed the required height!</t>
+  </si>
+  <si>
+    <t>unit_cube</t>
+  </si>
+  <si>
+    <t>Unit Cube</t>
+  </si>
+  <si>
+    <t>one_unit</t>
+  </si>
+  <si>
+    <t>1 Unit</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>cubic_unit_eval</t>
+  </si>
+  <si>
+    <t>1 Unit x 1 Unit x 1 Unit = 1 Cubic Unit</t>
+  </si>
+  <si>
+    <t>sides_eval</t>
+  </si>
+  <si>
+    <t>Sides: Length, Width, Height</t>
+  </si>
+  <si>
+    <t>volume_eval</t>
+  </si>
+  <si>
+    <t>Length x Width x Height = Volume</t>
+  </si>
+  <si>
+    <t>level_0_intro_1_3</t>
+  </si>
+  <si>
+    <t>level_0_intro_1_4</t>
+  </si>
+  <si>
+    <t>Remember that the volume of an object tells us how much it occupies space.</t>
+  </si>
+  <si>
+    <t>By using unit cubes, we can easily determine where to place the materials, and how much volume we will need.</t>
+  </si>
+  <si>
+    <t>level_0_intro_1_5</t>
+  </si>
+  <si>
+    <t>So if an object is made up of unit cubes, then the volume is equal to the number of unit cubes that make up the object.</t>
+  </si>
+  <si>
+    <t>A unit cube's measurement can also be changed based on specific needs. In our case, one unit cube equals to one cubic feet.</t>
+  </si>
+  <si>
+    <t>level_0_intro_2_0</t>
+  </si>
+  <si>
+    <t>Here's our first objective.</t>
+  </si>
+  <si>
+    <t>level_0_intro_2_1</t>
+  </si>
+  <si>
+    <t>You will be placing a number of unit cubes on the ground to match the required volume.</t>
+  </si>
+  <si>
+    <t>These buttons will allow you to rotate or elevate the view.</t>
+  </si>
+  <si>
+    <t>drag_material_instruct</t>
+  </si>
+  <si>
+    <t>drag_side_instruct</t>
+  </si>
+  <si>
+    <t>Press and drag the material to the designated location.</t>
+  </si>
+  <si>
+    <t>verify_instruct</t>
+  </si>
+  <si>
+    <t>expand_confirm_instruct</t>
+  </si>
+  <si>
+    <t>Press this button to finish expanding.</t>
+  </si>
+  <si>
+    <t>Press and drag the sides to expand the material.</t>
+  </si>
+  <si>
+    <t>build_instruct</t>
+  </si>
+  <si>
+    <t>Press this button to build.</t>
+  </si>
+  <si>
+    <t>Press here when you are ready to proceed.</t>
+  </si>
+  <si>
+    <t>Press this button to continue.</t>
   </si>
 </sst>
 </file>
@@ -628,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,26 +791,26 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,10 +973,10 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -897,18 +1008,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
         <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,7 +1027,7 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,7 +1035,7 @@
         <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,7 +1051,7 @@
         <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,85 +1059,232 @@
         <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>73</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks and such, more dialogs/etc., end stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C598F135-A39E-4EA6-8210-4C150E3B4F3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8FA683-6C76-4D16-9DE2-2FEE37FECFA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Key</t>
   </si>
@@ -349,12 +349,6 @@
     <t>By using unit cubes, we can easily determine where to place the materials, and how much volume we will need.</t>
   </si>
   <si>
-    <t>level_0_intro_1_5</t>
-  </si>
-  <si>
-    <t>So if an object is made up of unit cubes, then the volume is equal to the number of unit cubes that make up the object.</t>
-  </si>
-  <si>
     <t>A unit cube's measurement can also be changed based on specific needs. In our case, one unit cube equals to one cubic feet.</t>
   </si>
   <si>
@@ -404,6 +398,138 @@
   </si>
   <si>
     <t>Press this button to continue.</t>
+  </si>
+  <si>
+    <t>level_0_end_1</t>
+  </si>
+  <si>
+    <t>level_0_end_2</t>
+  </si>
+  <si>
+    <t>level_0_end_3</t>
+  </si>
+  <si>
+    <t>If you count the number of unit cubes placed on the ground, it tells you the volume of the object.</t>
+  </si>
+  <si>
+    <t>Anyhow, it's time to build!</t>
+  </si>
+  <si>
+    <t>In this case, this object is made up of 16 unit cubes, where each cube's volume is 1 cubic feet. Therefore the volume of the object is 16 cubic feet.</t>
+  </si>
+  <si>
+    <t>level_1_intro_0_1</t>
+  </si>
+  <si>
+    <t>level_1_intro_0_2</t>
+  </si>
+  <si>
+    <t>For this objective, we will have to stack more than one layer of cubes.</t>
+  </si>
+  <si>
+    <t>In order to increase the stack while expanding, simply highlight the top surface and drag upwards.</t>
+  </si>
+  <si>
+    <t>level_2_intro_0_1</t>
+  </si>
+  <si>
+    <t>level_2_intro_0_2</t>
+  </si>
+  <si>
+    <t>level_2_intro_0_3</t>
+  </si>
+  <si>
+    <t>Since we are dealing with measuring the volume using unit cubes, first you need to compute the number of unit cubes.</t>
+  </si>
+  <si>
+    <t>level_2_intro_0_4</t>
+  </si>
+  <si>
+    <t>level_2_unit_formula</t>
+  </si>
+  <si>
+    <t>2 Units x 2 Units x 2 Units = 8 Cubic Units</t>
+  </si>
+  <si>
+    <t>level_2_unit_to_volume</t>
+  </si>
+  <si>
+    <t>8 Cubic Units x 1/8 ft³ = 1 ft³</t>
+  </si>
+  <si>
+    <t>level_2_unit_volume</t>
+  </si>
+  <si>
+    <t>Cubic Unit Volume = 1/8 ft³</t>
+  </si>
+  <si>
+    <t>On this level, the unit cube's sides are half a foot with a volume of one-eighth cubic feet.</t>
+  </si>
+  <si>
+    <t>Then simply multiply the number of unit cubes with the unit cube's volume to get the correct result.</t>
+  </si>
+  <si>
+    <t>So for this level, we will need 8 unit cubes. Multiply 8 with one-eighth to convert it to the correct volume, which is 1 cubic foot.</t>
+  </si>
+  <si>
+    <t>level_4_intro_0_1</t>
+  </si>
+  <si>
+    <t>On this level, you will need to place two groups of unit cubes to get the required amount of volume.</t>
+  </si>
+  <si>
+    <t>level_4_intro_0_2</t>
+  </si>
+  <si>
+    <t>Volumes can be added together in any shape or form, so long as they are in the same measurement.</t>
+  </si>
+  <si>
+    <t>level_4_intro_0_3</t>
+  </si>
+  <si>
+    <t>In order for volumes to be added together make sure they are placed adjacently on any of the sides.</t>
+  </si>
+  <si>
+    <t>level_6_intro_0_1</t>
+  </si>
+  <si>
+    <t>On this level, one of the objectives have a restricted height.</t>
+  </si>
+  <si>
+    <t>level_6_intro_0_2</t>
+  </si>
+  <si>
+    <t>You won't be able to expand this particular material's height beyond the limit.</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>end_title</t>
+  </si>
+  <si>
+    <t>CONGRATULATIONS</t>
+  </si>
+  <si>
+    <t>end_detail</t>
+  </si>
+  <si>
+    <t>You have successfully given all the frogs a loving home!</t>
+  </si>
+  <si>
+    <t>end_detail_2</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>total_score</t>
+  </si>
+  <si>
+    <t>Total Score:</t>
   </si>
 </sst>
 </file>
@@ -739,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,492 +925,675 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>89</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>93</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>94</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>95</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>101</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>103</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>99</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>73</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>75</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48">
-        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+      <c r="C52">
+        <v>2.5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="C53">
+        <v>2.5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55">
-        <v>3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>114</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>143</v>
+      </c>
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some tweaks, build/submit stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67777F2-BD10-4ACA-A948-F905DF0BE395}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB172258-B262-4B1C-A7A5-671542F64F05}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1379,7 @@
         <v>80</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
         <v>112</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>158</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
some level tweaks, added level 4a, added delete all button
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB172258-B262-4B1C-A7A5-671542F64F05}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069CDF9A-4F61-4FDA-BB31-B31284F9DBBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9135" yWindow="2805" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Key</t>
   </si>
@@ -536,6 +536,42 @@
   </si>
   <si>
     <t>In order for volumes to be added together, make sure they are placed adjacently on any of the sides.</t>
+  </si>
+  <si>
+    <t>level_0_end_2_a</t>
+  </si>
+  <si>
+    <t>To simplify this, take the measurement of the length, width, and height; then multiply them. In this case: 4 times 4 times 1 equals 16.</t>
+  </si>
+  <si>
+    <t>delete_all_title</t>
+  </si>
+  <si>
+    <t>Delete All Cubes</t>
+  </si>
+  <si>
+    <t>delete_all_desc</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete all the cubes?</t>
+  </si>
+  <si>
+    <t>level_4_intro_0_4</t>
+  </si>
+  <si>
+    <t>Simply apply what you've done from the previous level to fill the grid, but with only one type of cube.</t>
   </si>
 </sst>
 </file>
@@ -871,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,155 +1495,203 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="B82" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83">
-        <v>1.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
-      </c>
-      <c r="C84">
-        <v>3.5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>155</v>
+      </c>
+      <c r="B85" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>157</v>
+      </c>
+      <c r="B86" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>159</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>160</v>
       </c>
-      <c r="C85">
+      <c r="C87">
         <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>